<commit_message>
xlsx conversion fix Unit 9 worksheet
</commit_message>
<xml_diff>
--- a/unit_8_9_worksheets/worksheets/Unit9_Charts_Worksheet.xlsx
+++ b/unit_8_9_worksheets/worksheets/Unit9_Charts_Worksheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -33,6 +33,59 @@
   </si>
   <si>
     <t>Table 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Exercise 9.1 Brandprefs</t>
+    </r>
+  </si>
+  <si>
+    <t>Exercise 9.5 Heather</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Exercise 9.5 Heather</t>
+    </r>
+  </si>
+  <si>
+    <t>Exercise 9.3 Diet A</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Exercise 9.3 Diet A</t>
+    </r>
+  </si>
+  <si>
+    <t>Exercise 9.6 Diet B</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="13"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Exercise 9.6 Diet B</t>
+    </r>
   </si>
   <si>
     <t>Brand</t>
@@ -66,9 +119,6 @@
     </r>
   </si>
   <si>
-    <t>Exercise 9.5 Heather</t>
-  </si>
-  <si>
     <t>Prevalence</t>
   </si>
   <si>
@@ -91,9 +141,6 @@
   </si>
   <si>
     <t>Location A is much richer; Location B has nearly half of transepts absent.</t>
-  </si>
-  <si>
-    <t>Exercise 9.3 Diet A</t>
   </si>
   <si>
     <t>Class Interval</t>
@@ -133,9 +180,6 @@
     </r>
   </si>
   <si>
-    <t>Exercise 9.6 Diet B</t>
-  </si>
-  <si>
     <t>(-6,-4]</t>
   </si>
   <si>
@@ -149,9 +193,19 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
@@ -166,19 +220,9 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
+      <color indexed="13"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -193,13 +237,18 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="18"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,12 +263,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,17 +284,128 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="10"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -248,42 +414,93 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -311,11 +528,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff878787"/>
       <rgbColor rgb="fff9f9f9"/>
     </indexedColors>
@@ -358,10 +575,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.272032"/>
+          <c:x val="0.196439"/>
           <c:y val="0"/>
-          <c:w val="0.455936"/>
-          <c:h val="0.128164"/>
+          <c:w val="0.607122"/>
+          <c:h val="0.177755"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -377,10 +594,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.168874"/>
-          <c:y val="0.128164"/>
-          <c:w val="0.826126"/>
-          <c:h val="0.76326"/>
+          <c:x val="0.224872"/>
+          <c:y val="0.177755"/>
+          <c:w val="0.770128"/>
+          <c:h val="0.688171"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -573,7 +790,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
@@ -681,8 +898,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
-        <c:minorUnit val="10"/>
+        <c:majorUnit val="25"/>
+        <c:minorUnit val="12.5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -749,10 +966,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.146735"/>
+          <c:x val="0.0667124"/>
           <c:y val="0"/>
-          <c:w val="0.706531"/>
-          <c:h val="0.135439"/>
+          <c:w val="0.865738"/>
+          <c:h val="0.213877"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -768,10 +985,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0906152"/>
-          <c:y val="0.135439"/>
-          <c:w val="0.904385"/>
-          <c:h val="0.748751"/>
+          <c:x val="0.138981"/>
+          <c:y val="0.213877"/>
+          <c:w val="0.856019"/>
+          <c:h val="0.671938"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1015,6 +1232,7 @@
         <c:axId val="2094734553"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1059,8 +1277,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="15"/>
-        <c:minorUnit val="7.5"/>
+        <c:majorUnit val="25"/>
+        <c:minorUnit val="12.5"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1079,10 +1297,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0906152"/>
-          <c:y val="0.0677196"/>
-          <c:w val="0.9"/>
-          <c:h val="0.0927196"/>
+          <c:x val="0.114836"/>
+          <c:y val="0.141405"/>
+          <c:w val="0.885164"/>
+          <c:h val="0.0916537"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1163,10 +1381,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.209581"/>
+          <c:x val="0.216308"/>
           <c:y val="0"/>
-          <c:w val="0.580837"/>
-          <c:h val="0.135439"/>
+          <c:w val="0.562384"/>
+          <c:h val="0.13889"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1182,10 +1400,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.156141"/>
-          <c:y val="0.135439"/>
-          <c:w val="0.838859"/>
-          <c:h val="0.748751"/>
+          <c:x val="0.182949"/>
+          <c:y val="0.13889"/>
+          <c:w val="0.812051"/>
+          <c:h val="0.742668"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1502,8 +1720,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="10"/>
-        <c:minorUnit val="5"/>
+        <c:majorUnit val="12.5"/>
+        <c:minorUnit val="6.25"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1522,10 +1740,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.132377"/>
-          <c:y val="0.0677196"/>
-          <c:w val="0.867623"/>
-          <c:h val="0.0927196"/>
+          <c:x val="0.15994"/>
+          <c:y val="0.0631154"/>
+          <c:w val="0.84006"/>
+          <c:h val="0.0944448"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1606,10 +1824,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16493"/>
+          <c:x val="0.161554"/>
           <c:y val="0"/>
-          <c:w val="0.67014"/>
-          <c:h val="0.0951298"/>
+          <c:w val="0.676892"/>
+          <c:h val="0.115407"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1625,10 +1843,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.204238"/>
-          <c:y val="0.0951298"/>
-          <c:w val="0.790762"/>
-          <c:h val="0.664882"/>
+          <c:x val="0.206296"/>
+          <c:y val="0.115407"/>
+          <c:w val="0.788704"/>
+          <c:h val="0.603696"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1882,7 +2100,7 @@
           <c:overlay val="1"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
@@ -2057,10 +2275,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.133689"/>
+          <c:x val="0.129374"/>
           <c:y val="0"/>
-          <c:w val="0.732622"/>
-          <c:h val="0.115294"/>
+          <c:w val="0.741252"/>
+          <c:h val="0.134799"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -2076,10 +2294,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12756"/>
-          <c:y val="0.115294"/>
-          <c:w val="0.86744"/>
-          <c:h val="0.685364"/>
+          <c:x val="0.152678"/>
+          <c:y val="0.134799"/>
+          <c:w val="0.842322"/>
+          <c:h val="0.643108"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -2326,7 +2544,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
         <c:spPr>
@@ -2405,8 +2623,8 @@
         <c:crossAx val="2094734552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="0.05"/>
-        <c:minorUnit val="0.025"/>
+        <c:majorUnit val="0.0875"/>
+        <c:minorUnit val="0.04375"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2443,15 +2661,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76023</xdr:rowOff>
+      <xdr:colOff>26542</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>123711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>554533</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>36945</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>543135</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>89238</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2459,8 +2677,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="-478334" y="1742263"/>
-        <a:ext cx="5558334" cy="3770923"/>
+        <a:off x="26542" y="1581036"/>
+        <a:ext cx="4174194" cy="2718888"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2473,15 +2691,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>60152</xdr:rowOff>
+      <xdr:colOff>42553</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152915</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>9005</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>530754</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>164545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2489,8 +2707,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="6298392"/>
-        <a:ext cx="5080001" cy="3568354"/>
+        <a:off x="42553" y="4191515"/>
+        <a:ext cx="4145802" cy="3625416"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2508,15 +2726,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>81638</xdr:rowOff>
+      <xdr:colOff>69325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>96257</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>291169</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>30490</xdr:rowOff>
+      <xdr:colOff>533398</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>134261</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2524,8 +2742,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="-189570" y="2041248"/>
-        <a:ext cx="5269571" cy="3568353"/>
+        <a:off x="69325" y="1465952"/>
+        <a:ext cx="5442474" cy="3479705"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2543,15 +2761,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>118117</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>15180</xdr:rowOff>
+      <xdr:rowOff>563</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>464070</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>142552</xdr:rowOff>
+      <xdr:colOff>527902</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>58260</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2559,8 +2777,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="-362471" y="2447230"/>
-        <a:ext cx="5442471" cy="5080373"/>
+        <a:off x="118117" y="2395783"/>
+        <a:ext cx="5388186" cy="4187738"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2578,15 +2796,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>115862</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>82175</xdr:rowOff>
+      <xdr:colOff>93548</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>83007</xdr:rowOff>
+      <xdr:colOff>554892</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>143893</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2594,8 +2812,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="115862" y="3239395"/>
-        <a:ext cx="4964138" cy="4191833"/>
+        <a:off x="93548" y="2567588"/>
+        <a:ext cx="4906345" cy="3585311"/>
       </xdr:xfrm>
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2753,9 +2971,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -2835,7 +3053,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2862,10 +3080,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3112,9 +3330,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -3392,7 +3610,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -3419,10 +3637,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3664,96 +3882,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="4" width="30.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="0.05" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" ht="8" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="17.9" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="15.35" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="15.35" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
+      <c r="D10" t="s" s="14">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="15.35" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="15.35" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="12"/>
+      <c r="C12" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D12" t="s" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="4"/>
-      <c r="C14" t="s" s="4">
+      <c r="D12" t="s" s="14">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" ht="15.35" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s" s="10">
+        <v>9</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" ht="15.35" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="12"/>
+      <c r="C14" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D14" t="s" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="s" s="3">
-        <v>34</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="4"/>
-      <c r="C16" t="s" s="4">
+      <c r="D14" t="s" s="14">
+        <v>10</v>
+      </c>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" ht="15.35" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" ht="15.35" customHeight="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" t="s" s="17">
         <v>5</v>
       </c>
-      <c r="D16" t="s" s="5">
-        <v>34</v>
-      </c>
+      <c r="D16" t="s" s="18">
+        <v>12</v>
+      </c>
+      <c r="E16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3765,91 +4051,414 @@
     <hyperlink ref="D14" location="'Exercise 9.3 Diet A'!R1C1" tooltip="" display="Exercise 9.3 Diet A"/>
     <hyperlink ref="D16" location="'Exercise 9.6 Diet B'!R1C1" tooltip="" display="Exercise 9.6 Diet B"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.6719" style="6" customWidth="1"/>
-    <col min="2" max="5" width="8.85156" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.6719" style="20" customWidth="1"/>
+    <col min="2" max="6" width="8.85156" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>8</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" t="s" s="21">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s" s="21">
+        <v>15</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>9</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" t="s" s="21">
+        <v>16</v>
+      </c>
+      <c r="B2" s="24">
         <v>15.7</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="24">
         <v>21.1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" t="s" s="21">
+        <v>17</v>
+      </c>
+      <c r="B3" s="24">
         <v>24.3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="24">
         <v>33.3</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>11</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" t="s" s="21">
+        <v>18</v>
+      </c>
+      <c r="B4" s="24">
         <v>60</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="24">
         <v>45.6</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="25"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" ht="33.45" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" t="s" s="26">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="27">
+        <v>20</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" ht="13.55" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" ht="13.55" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" ht="13.55" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" ht="13.55" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" ht="13.55" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" ht="13.55" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" ht="13.55" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" ht="13.55" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" ht="13.55" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" ht="13.55" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" ht="13.55" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" ht="13.55" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" ht="13.55" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" ht="13.55" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" ht="13.55" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" ht="13.55" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" ht="13.55" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" ht="13.55" customHeight="1">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" ht="13.55" customHeight="1">
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" ht="13.55" customHeight="1">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" ht="13.55" customHeight="1">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" ht="13.55" customHeight="1">
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" ht="13.55" customHeight="1">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" ht="13.55" customHeight="1">
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" ht="13.55" customHeight="1">
+      <c r="A45" s="15"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3866,86 +4475,344 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.3516" style="12" customWidth="1"/>
-    <col min="2" max="5" width="8.85156" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.3516" style="29" customWidth="1"/>
+    <col min="2" max="8" width="8.85156" style="29" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" t="s" s="21">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s" s="21">
+        <v>23</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" t="s" s="21">
+        <v>24</v>
+      </c>
+      <c r="B2" s="24">
         <v>14.3</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="24">
         <v>45.5</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" t="s" s="21">
+        <v>25</v>
+      </c>
+      <c r="B3" s="24">
         <v>39.3</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="24">
         <v>31.8</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" t="s" s="21">
+        <v>26</v>
+      </c>
+      <c r="B4" s="24">
         <v>46.4</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="24">
         <v>22.7</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" ht="26.55" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="A6" t="s" s="26">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s" s="27">
+        <v>28</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" ht="13.55" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" ht="13.55" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" ht="13.55" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" ht="13.55" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" ht="13.55" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" ht="13.55" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" ht="13.55" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" ht="13.55" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" ht="13.55" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" ht="13.55" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" ht="13.55" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" ht="13.55" customHeight="1">
+      <c r="A30" s="15"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3962,122 +4829,432 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.3516" style="13" customWidth="1"/>
-    <col min="2" max="5" width="8.85156" style="13" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="13" customWidth="1"/>
+    <col min="1" max="1" width="12.3516" style="30" customWidth="1"/>
+    <col min="2" max="8" width="8.85156" style="30" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" t="s" s="21">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>30</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" t="s" s="21">
+        <v>31</v>
+      </c>
+      <c r="B2" s="24">
         <v>0.02</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="7">
+      <c r="A3" t="s" s="21">
+        <v>32</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="21">
+        <v>33</v>
+      </c>
+      <c r="B4" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="21">
+        <v>34</v>
+      </c>
+      <c r="B5" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="21">
+        <v>35</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="21">
+        <v>36</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="21">
+        <v>37</v>
+      </c>
+      <c r="B8" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" ht="39.55" customHeight="1">
+      <c r="A10" t="s" s="26">
         <v>27</v>
       </c>
-      <c r="B3" s="9">
-        <v>0.06</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="39.55" customHeight="1">
-      <c r="A10" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" t="s" s="27">
+        <v>38</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" ht="13.55" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" ht="13.55" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" ht="13.55" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" ht="13.55" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" ht="13.55" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" ht="13.55" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" ht="13.55" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" ht="13.55" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" ht="13.55" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" ht="13.55" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" ht="13.55" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" ht="13.55" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" ht="13.55" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" ht="13.55" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" ht="13.55" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" ht="13.55" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" ht="13.55" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" ht="13.55" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" ht="13.55" customHeight="1">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" ht="13.55" customHeight="1">
+      <c r="A38" s="15"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4094,145 +5271,385 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.3516" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.6094" style="14" customWidth="1"/>
-    <col min="3" max="5" width="8.85156" style="14" customWidth="1"/>
-    <col min="6" max="16384" width="8.85156" style="14" customWidth="1"/>
+    <col min="1" max="1" width="12.3516" style="31" customWidth="1"/>
+    <col min="2" max="2" width="10.6719" style="31" customWidth="1"/>
+    <col min="3" max="7" width="8.85156" style="31" customWidth="1"/>
+    <col min="8" max="16384" width="8.85156" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>25</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" t="s" s="21">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s" s="21">
+        <v>30</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="7">
+      <c r="A2" t="s" s="21">
+        <v>39</v>
+      </c>
+      <c r="B2" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" t="s" s="21">
+        <v>40</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" t="s" s="21">
+        <v>31</v>
+      </c>
+      <c r="B4" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" t="s" s="21">
+        <v>32</v>
+      </c>
+      <c r="B5" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" t="s" s="21">
+        <v>33</v>
+      </c>
+      <c r="B6" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" t="s" s="21">
+        <v>34</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.22</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" t="s" s="21">
         <v>35</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B8" s="24">
+        <v>0.16</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" t="s" s="21">
+        <v>36</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.04</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" t="s" s="21">
+        <v>37</v>
+      </c>
+      <c r="B10" s="24">
         <v>0.02</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="B3" s="9">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="B4" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="7">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" ht="13.55" customHeight="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" ht="39.55" customHeight="1">
+      <c r="A12" t="s" s="26">
         <v>27</v>
       </c>
-      <c r="B5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0.3</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0.22</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="B8" s="9">
-        <v>0.16</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0.04</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" ht="39.55" customHeight="1">
-      <c r="A12" t="s" s="10">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="B12" t="s" s="27">
+        <v>38</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" ht="13.55" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" ht="13.55" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" ht="13.55" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" ht="13.55" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" ht="13.55" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" ht="13.55" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" ht="13.55" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" ht="13.55" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" ht="13.55" customHeight="1">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" ht="13.55" customHeight="1">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" ht="13.55" customHeight="1">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" ht="13.55" customHeight="1">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" ht="13.55" customHeight="1">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" ht="13.55" customHeight="1">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" ht="13.55" customHeight="1">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" ht="13.55" customHeight="1">
+      <c r="A28" s="5"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" ht="13.55" customHeight="1">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" ht="13.55" customHeight="1">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" ht="13.55" customHeight="1">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" ht="13.55" customHeight="1">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" ht="13.55" customHeight="1">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" ht="13.55" customHeight="1">
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" ht="13.55" customHeight="1">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" ht="13.55" customHeight="1">
+      <c r="A36" s="15"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>